<commit_message>
create a scrum tab. Review agenda
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/fullstack_mars_2024/10_final_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B29290C6-611C-40FE-B402-CEABF40DE66B}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA9E27CD-C2E5-42A5-8461-BC1BCC181C38}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Agenda" sheetId="1" r:id="rId1"/>
+    <sheet name="SCRUM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -108,76 +109,6 @@
   </si>
   <si>
     <t>CODE 3/3</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>17H30</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> : demo/POC - Inviter le prof ?
-Faire le point sur : 
- - ce qu'on a
- - ce qui nous manque
- - …</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>12H00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> : demo/POC  - Inviter le prof ?
-Faire le point sur : 
- - ce qu'on a
- - ce qui nous manque
- - …
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>18H00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> : Fournir les données, graphes, captures écrans pour les slides</t>
-    </r>
   </si>
   <si>
     <r>
@@ -277,6 +208,107 @@
   </si>
   <si>
     <t>Remain</t>
+  </si>
+  <si>
+    <t>Dominique</t>
+  </si>
+  <si>
+    <t>Patrice</t>
+  </si>
+  <si>
+    <t>Philippe</t>
+  </si>
+  <si>
+    <t>Yesterday</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>Quentin</t>
+  </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>12H00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : demo/POC  - Inviter le prof
+Faire le point sur : 
+ - ce qu'on a
+ - ce qui nous manque
+ - …
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>18H00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : Fournir les données, graphes, captures écrans pour les slides</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>10H00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : Après le SCRUM meeting - demo/POC - Inviter le prof
+Faire le point sur : 
+ - ce qu'on a
+ - ce qui nous manque
+ - …</t>
+    </r>
+  </si>
+  <si>
+    <t>Lost of persistence on the server ?</t>
+  </si>
+  <si>
+    <t>Architecture study
+Course review</t>
+  </si>
+  <si>
+    <t>Finish course review</t>
   </si>
 </sst>
 </file>
@@ -322,7 +354,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,6 +397,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -633,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -671,12 +709,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -685,21 +717,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -734,6 +751,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1466,8 +1552,88 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>183606</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>132806</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6093976" cy="441018"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5315467-F9EE-F87B-A25B-3BAFC88DD043}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="183606" y="132806"/>
+          <a:ext cx="6093976" cy="441018"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="10000"/>
+            <a:lumOff val="90000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Feel free to read :   </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="fr-FR" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1200">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>https://ignition-program.com/tuto/la-methode-scrum-pour-les-nuls</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1789,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C2E7AC-1286-4FC1-84B0-DB92C81B15DE}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1805,13 +1971,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
-        <v>22</v>
+      <c r="A2" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="25" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -1822,10 +1988,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="35">
+      <c r="A3" s="28">
         <v>18</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="26">
         <v>45442</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1837,10 +2003,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="36">
+      <c r="A4" s="29">
         <v>17</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="19">
         <v>45443</v>
       </c>
       <c r="C4" s="1"/>
@@ -1850,10 +2016,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="36">
+      <c r="A5" s="29">
         <v>16</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="19">
         <v>45444</v>
       </c>
       <c r="C5" s="2"/>
@@ -1863,10 +2029,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="36">
+      <c r="A6" s="29">
         <v>15</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="19">
         <v>45445</v>
       </c>
       <c r="C6" s="2"/>
@@ -1876,178 +2042,178 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="216" x14ac:dyDescent="0.3">
-      <c r="A7" s="36">
+      <c r="A7" s="29">
         <v>14</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="19">
         <v>45446</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="11"/>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
+      <c r="A8" s="20">
         <v>13</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="19">
         <v>45447</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>21</v>
+      <c r="E8" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="27">
+      <c r="A9" s="20">
         <v>12</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="19">
         <v>45448</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="28"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
+      <c r="A10" s="20">
         <v>11</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="19">
         <v>45449</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="22"/>
     </row>
     <row r="11" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27">
+      <c r="A11" s="20">
         <v>10</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="19">
         <v>45450</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="D11" s="32"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="20">
         <v>9</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="19">
         <v>45451</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="16" t="s">
-        <v>16</v>
-      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="27">
+      <c r="A13" s="20">
         <v>8</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="19">
         <v>45452</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
+      <c r="A14" s="20">
         <v>7</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="19">
         <v>45453</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27">
+      <c r="D14" s="33"/>
+      <c r="E14" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20">
         <v>6</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="19">
         <v>45454</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="17"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
+      <c r="A16" s="20">
         <v>5</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="19">
         <v>45455</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="23"/>
+      <c r="E16" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="27">
+      <c r="A17" s="20">
         <v>4</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="19">
         <v>45456</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="24"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="20">
         <v>3</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B18" s="19">
         <v>45457</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23" t="s">
-        <v>17</v>
+      <c r="D18" s="36"/>
+      <c r="E18" s="16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="27">
+      <c r="A19" s="20">
         <v>2</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="19">
         <v>45458</v>
       </c>
       <c r="C19" s="2"/>
@@ -2057,10 +2223,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="27">
+      <c r="A20" s="20">
         <v>1</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="19">
         <v>45459</v>
       </c>
       <c r="C20" s="2"/>
@@ -2070,20 +2236,20 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="30">
+      <c r="A21" s="23">
         <v>0</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="24">
         <v>45460</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="25" t="s">
-        <v>19</v>
+      <c r="D21" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2097,4 +2263,338 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
+  <dimension ref="A5:M20"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="32.88671875" customWidth="1"/>
+    <col min="9" max="9" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="37">
+        <v>45447</v>
+      </c>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="37">
+        <v>45448</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="37">
+        <v>45449</v>
+      </c>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="37">
+        <v>45450</v>
+      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
+        <v>45451</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>45452</v>
+      </c>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="37">
+        <v>45453</v>
+      </c>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="37">
+        <v>45454</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="37">
+        <v>45455</v>
+      </c>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="37">
+        <v>45456</v>
+      </c>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="37">
+        <v>45457</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="38">
+        <v>45458</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="38">
+        <v>45459</v>
+      </c>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="37">
+        <v>45460</v>
+      </c>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updtate suite reunion Aurélie
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA9E27CD-C2E5-42A5-8461-BC1BCC181C38}"/>
+  <xr:revisionPtr revIDLastSave="217" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35E116E9-A736-488F-9230-33BC5B7A67F8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -46,15 +46,6 @@
   </si>
   <si>
     <t>Due</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Présentation l'après midi </t>
-  </si>
-  <si>
-    <t>Terminer les slides à midi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCRUM du matin </t>
   </si>
   <si>
     <t>Recherche dataset, technique, fesabilité…</t>
@@ -68,9 +59,6 @@
   </si>
   <si>
     <t>SPRINT</t>
-  </si>
-  <si>
-    <t>DOC</t>
   </si>
   <si>
     <t>Finalisation des slides</t>
@@ -189,22 +177,6 @@
         * pour quelle date?    Jusqu'à Mercredi soir
   </t>
     </r>
-  </si>
-  <si>
-    <t>Faire un github
-Faire un point GitHub - Bonnes pratiques
-Slides
-  Site Web &amp; API
-  Dataset &amp; modèle
-  Transfer Learning
-  archi…
-Si il y a des échanges entre telle ou telle partie
-    - quel format ?
-    - quelle API? 
-    - confirmer les livrables
-Confirmer l'architecture du projet
-Si 2 jours c'est trop =&gt; Commencer un POC
-Pourra servir pour la documentation du projet</t>
   </si>
   <si>
     <t>Remain</t>
@@ -276,6 +248,45 @@
     </r>
   </si>
   <si>
+    <t>Lost of persistence on the server ?</t>
+  </si>
+  <si>
+    <t>Architecture study
+Course review</t>
+  </si>
+  <si>
+    <t>Finish course review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peau saine
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>10H45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : Après le point Aurélie - demo/POC - Inviter le prof
+Faire le point sur : 
+ - ce qu'on a
+ - ce qui nous manque
+ - …</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -293,7 +304,7 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> : Après le SCRUM meeting - demo/POC - Inviter le prof
+      <t xml:space="preserve"> : Après le point Aurélie - demo/POC - Inviter le prof
 Faire le point sur : 
  - ce qu'on a
  - ce qui nous manque
@@ -301,14 +312,59 @@
     </r>
   </si>
   <si>
-    <t>Lost of persistence on the server ?</t>
-  </si>
-  <si>
-    <t>Architecture study
-Course review</t>
-  </si>
-  <si>
-    <t>Finish course review</t>
+    <r>
+      <t xml:space="preserve">DONE - Faire un github - Quentin
+DONE - Serveur Discord - Quentin
+Faire un point GitHub - Bonnes pratiques - Quentin
+Suite doc, faire un ou 2 slides de présentation pour </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">jeudi 6?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Mettre ses idées à plat, les présenter à l'équipe
+  Site Web &amp; API     - Quentin
+  Dataset &amp; modèle   - Dominique
+  Transfer Learning  - Patrice
+  Archi              - Philippe
+Si il y a des échanges entre telle ou telle partie
+En discuter jeudi après les synthèses slides
+    - quel format ?
+    - quelle API? 
+    - confirmer les livrables
+Si 2 jours c'est trop =&gt; Commencer un POC
+Pourra servir pour la documentation du projet</t>
+    </r>
+  </si>
+  <si>
+    <t>DOC-VEILLE</t>
+  </si>
+  <si>
+    <t>09h30 - Point Aurélie 
+10H00 - SCRUM du matin</t>
+  </si>
+  <si>
+    <t>09h30 - Point Aurélie 
+10H00 - SCRUM du matin AurélieTerminer l'archi des slides à midi?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09h30 - Point Aurélie 
+10H00 - SCRUM du matin
+Présentation l'après midi </t>
   </si>
 </sst>
 </file>
@@ -354,7 +410,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +459,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -671,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -681,9 +743,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -752,6 +811,42 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -773,12 +868,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -792,33 +881,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -848,8 +919,8 @@
       <xdr:rowOff>1714501</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>277907</xdr:rowOff>
     </xdr:to>
@@ -866,8 +937,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12672956" y="3910854"/>
-          <a:ext cx="10233362" cy="5502088"/>
+          <a:off x="12870180" y="3910854"/>
+          <a:ext cx="10438055" cy="5681382"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1634,6 +1705,10 @@
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1955,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C2E7AC-1286-4FC1-84B0-DB92C81B15DE}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="127" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1971,285 +2046,285 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="27">
+        <v>18</v>
+      </c>
+      <c r="B3" s="25">
+        <v>45442</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="7" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="28">
+        <v>17</v>
+      </c>
+      <c r="B4" s="18">
+        <v>45443</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="28">
+        <v>16</v>
+      </c>
+      <c r="B5" s="18">
+        <v>45444</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="55" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="28">
+        <v>15</v>
+      </c>
+      <c r="B6" s="18">
+        <v>45445</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="55" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+      <c r="A7" s="28">
+        <v>14</v>
+      </c>
+      <c r="B7" s="18">
+        <v>45446</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A8" s="28">
+        <v>13</v>
+      </c>
+      <c r="B8" s="18">
+        <v>45447</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="19">
+        <v>12</v>
+      </c>
+      <c r="B9" s="18">
+        <v>45448</v>
+      </c>
+      <c r="C9" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19">
+        <v>11</v>
+      </c>
+      <c r="B10" s="18">
+        <v>45449</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="18">
+        <v>45450</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="19">
+        <v>9</v>
+      </c>
+      <c r="B12" s="18">
+        <v>45451</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="55"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="19">
+        <v>8</v>
+      </c>
+      <c r="B13" s="18">
+        <v>45452</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="55"/>
+    </row>
+    <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="19">
+        <v>7</v>
+      </c>
+      <c r="B14" s="18">
+        <v>45453</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19">
+        <v>6</v>
+      </c>
+      <c r="B15" s="18">
+        <v>45454</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="19">
+        <v>5</v>
+      </c>
+      <c r="B16" s="18">
+        <v>45455</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="19">
+        <v>4</v>
+      </c>
+      <c r="B17" s="18">
+        <v>45456</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="19">
+        <v>3</v>
+      </c>
+      <c r="B18" s="18">
+        <v>45457</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="19">
+        <v>2</v>
+      </c>
+      <c r="B19" s="18">
+        <v>45458</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="28">
-        <v>18</v>
-      </c>
-      <c r="B3" s="26">
-        <v>45442</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="6" t="s">
+      <c r="B20" s="18">
+        <v>45459</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="22">
+        <v>0</v>
+      </c>
+      <c r="B21" s="23">
+        <v>45460</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="29">
-        <v>17</v>
-      </c>
-      <c r="B4" s="19">
-        <v>45443</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="29">
-        <v>16</v>
-      </c>
-      <c r="B5" s="19">
-        <v>45444</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="29">
-        <v>15</v>
-      </c>
-      <c r="B6" s="19">
-        <v>45445</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="216" x14ac:dyDescent="0.3">
-      <c r="A7" s="29">
-        <v>14</v>
-      </c>
-      <c r="B7" s="19">
-        <v>45446</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="20">
-        <v>13</v>
-      </c>
-      <c r="B8" s="19">
-        <v>45447</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
-        <v>12</v>
-      </c>
-      <c r="B9" s="19">
-        <v>45448</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20">
-        <v>11</v>
-      </c>
-      <c r="B10" s="19">
-        <v>45449</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20">
-        <v>10</v>
-      </c>
-      <c r="B11" s="19">
-        <v>45450</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="20">
-        <v>9</v>
-      </c>
-      <c r="B12" s="19">
-        <v>45451</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="20">
-        <v>8</v>
-      </c>
-      <c r="B13" s="19">
-        <v>45452</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="20">
-        <v>7</v>
-      </c>
-      <c r="B14" s="19">
-        <v>45453</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20">
-        <v>6</v>
-      </c>
-      <c r="B15" s="19">
-        <v>45454</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20">
-        <v>5</v>
-      </c>
-      <c r="B16" s="19">
-        <v>45455</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="20">
-        <v>4</v>
-      </c>
-      <c r="B17" s="19">
-        <v>45456</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="20">
-        <v>3</v>
-      </c>
-      <c r="B18" s="19">
-        <v>45457</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="20">
-        <v>2</v>
-      </c>
-      <c r="B19" s="19">
-        <v>45458</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="20">
-        <v>1</v>
-      </c>
-      <c r="B20" s="19">
-        <v>45459</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23">
-        <v>0</v>
-      </c>
-      <c r="B21" s="24">
-        <v>45460</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2270,7 +2345,7 @@
   <dimension ref="A5:M20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2284,308 +2359,310 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="40" t="s">
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="42" t="s">
+      <c r="D6" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="29">
+        <v>45447</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="46" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="37">
-        <v>45447</v>
-      </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="37">
+      <c r="A8" s="29">
         <v>45448</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="37">
+      <c r="A9" s="29">
         <v>45449</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="37">
+      <c r="A10" s="29">
         <v>45450</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="38">
+      <c r="A11" s="30">
         <v>45451</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="38">
+      <c r="A12" s="30">
         <v>45452</v>
       </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="37">
+      <c r="A13" s="29">
         <v>45453</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="37">
+      <c r="A14" s="29">
         <v>45454</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="37">
+      <c r="A15" s="29">
         <v>45455</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="37">
+      <c r="A16" s="29">
         <v>45456</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="37">
+      <c r="A17" s="29">
         <v>45457</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="38">
+      <c r="A18" s="30">
         <v>45458</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="38">
+      <c r="A19" s="30">
         <v>45459</v>
       </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="37">
+      <c r="A20" s="29">
         <v>45460</v>
       </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Update suite SCRUM du jour
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="227" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98E48D33-00F4-4608-BA97-5F2878B71B0E}"/>
+  <xr:revisionPtr revIDLastSave="251" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB10F927-C06F-48C7-9484-34224B7871A0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -258,10 +258,6 @@
     <t>Finish course review</t>
   </si>
   <si>
-    <t xml:space="preserve">Peau saine
-</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -381,6 +377,46 @@
     <t xml:space="preserve">09h30 - Point Aurélie - Dominique
 10H00 - SCRUM du matin
 Présentation l'après midi </t>
+  </si>
+  <si>
+    <t>Peau saine
+Stockage des données. S3? 
+TO DO : réponse Philippe</t>
+  </si>
+  <si>
+    <t>Doc &amp; Veille</t>
+  </si>
+  <si>
+    <t>Revoir les cours. 
+Deep - Classification images</t>
+  </si>
+  <si>
+    <t>No problemo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No problemo
+</t>
+  </si>
+  <si>
+    <t>Veille. Papiers. Site HAL
+CNN
+Y a de quoi faire
+VGG16</t>
+  </si>
+  <si>
+    <t>Reprendre les cours
+Classi multimodal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github
+</t>
+  </si>
+  <si>
+    <t>Revoir cours
+API avec python
+Outil pour faire l'application
+2 fonctions
+Bouton Web App</t>
   </si>
 </sst>
 </file>
@@ -749,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -907,6 +943,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2046,7 +2088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C2E7AC-1286-4FC1-84B0-DB92C81B15DE}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="127" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="127" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2153,16 +2195,16 @@
         <v>45447</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>12</v>
       </c>
@@ -2170,7 +2212,7 @@
         <v>45448</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="46"/>
       <c r="E9" s="20"/>
@@ -2183,7 +2225,7 @@
         <v>45449</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="47" t="s">
         <v>10</v>
@@ -2198,7 +2240,7 @@
         <v>45450</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="13"/>
@@ -2235,11 +2277,11 @@
         <v>45453</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="48"/>
       <c r="E14" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
@@ -2250,7 +2292,7 @@
         <v>45454</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="48"/>
       <c r="E15" s="14"/>
@@ -2263,13 +2305,13 @@
         <v>45455</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="49" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2280,7 +2322,7 @@
         <v>45456</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="50"/>
       <c r="E17" s="16"/>
@@ -2293,7 +2335,7 @@
         <v>45457</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="51"/>
       <c r="E18" s="15" t="s">
@@ -2334,7 +2376,7 @@
         <v>45460</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>13</v>
@@ -2360,18 +2402,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.6640625" customWidth="1"/>
     <col min="8" max="8" width="32.88671875" customWidth="1"/>
     <col min="9" max="9" width="44.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="20.6640625" customWidth="1"/>
+    <col min="11" max="12" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="68.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2434,18 +2481,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>45447</v>
       </c>
-      <c r="B7" s="35"/>
+      <c r="B7" s="35" t="s">
+        <v>39</v>
+      </c>
       <c r="C7" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
+        <v>38</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>44</v>
+      </c>
       <c r="H7" s="40" t="s">
         <v>25</v>
       </c>
@@ -2455,9 +2512,15 @@
       <c r="J7" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
+      <c r="K7" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="57" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="29">

</xml_diff>

<commit_message>
Suite meeting table avec aurélie. Filigrane
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB10F927-C06F-48C7-9484-34224B7871A0}"/>
+  <xr:revisionPtr revIDLastSave="252" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69697815-558A-43B9-852E-2476EF2557A6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
@@ -379,11 +379,6 @@
 Présentation l'après midi </t>
   </si>
   <si>
-    <t>Peau saine
-Stockage des données. S3? 
-TO DO : réponse Philippe</t>
-  </si>
-  <si>
     <t>Doc &amp; Veille</t>
   </si>
   <si>
@@ -417,6 +412,12 @@
 Outil pour faire l'application
 2 fonctions
 Bouton Web App</t>
+  </si>
+  <si>
+    <t>Peau saine
+Stockage des données. S3? 
+TO DO : réponse Philippe
+On fait le test avec filigrane</t>
   </si>
 </sst>
 </file>
@@ -911,6 +912,12 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -943,12 +950,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2197,7 +2198,7 @@
       <c r="C8" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="47" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="12" t="s">
@@ -2214,7 +2215,7 @@
       <c r="C9" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="46"/>
+      <c r="D9" s="48"/>
       <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2227,7 +2228,7 @@
       <c r="C10" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="49" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="21"/>
@@ -2242,7 +2243,7 @@
       <c r="C11" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2253,7 +2254,7 @@
         <v>45451</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="47"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2264,7 +2265,7 @@
         <v>45452</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="50" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="44"/>
@@ -2279,7 +2280,7 @@
       <c r="C14" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="48"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="14" t="s">
         <v>27</v>
       </c>
@@ -2294,7 +2295,7 @@
       <c r="C15" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="48"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2307,7 +2308,7 @@
       <c r="C16" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="51" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="15" t="s">
@@ -2324,7 +2325,7 @@
       <c r="C17" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="50"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
@@ -2337,7 +2338,7 @@
       <c r="C18" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="51"/>
+      <c r="D18" s="53"/>
       <c r="E18" s="15" t="s">
         <v>23</v>
       </c>
@@ -2402,8 +2403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2422,26 +2423,26 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53" t="s">
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="54" t="s">
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="55" t="s">
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="31" t="s">
@@ -2481,27 +2482,27 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>45447</v>
       </c>
       <c r="B7" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="56" t="s">
+      <c r="E7" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="45" t="s">
         <v>43</v>
-      </c>
-      <c r="F7" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>44</v>
       </c>
       <c r="H7" s="40" t="s">
         <v>25</v>
@@ -2512,14 +2513,14 @@
       <c r="J7" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="57" t="s">
+      <c r="K7" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="46" t="s">
         <v>45</v>
-      </c>
-      <c r="L7" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="57" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update suite meeting scrum du jour
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E089B23-EEA1-4977-87ED-5AD7A10EFB69}"/>
+  <xr:revisionPtr revIDLastSave="312" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A1630C4-4D3D-42F1-97CF-845D09EFBD1E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -305,45 +305,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">DONE - Faire un github - Quentin
-DONE - Serveur Discord - Quentin
-Faire un point GitHub - Bonnes pratiques - Quentin
-Suite doc, faire un ou 2 slides de présentation pour </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">jeudi 6?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>Mettre ses idées à plat, les présenter à l'équipe
-  Site Web &amp; API     - Quentin
-  Dataset &amp; modèle   - Dominique
-  Transfer Learning  - Patrice
-  Archi              - Philippe
-Si il y a des échanges entre telle ou telle partie
-En discuter jeudi après les synthèses slides
-    - quel format ?
-    - quelle API? 
-    - confirmer les livrables
-Si 2 jours c'est trop =&gt; Commencer un POC
-Pourra servir pour la documentation du projet</t>
-    </r>
-  </si>
-  <si>
     <t>DOC-VEILLE</t>
   </si>
   <si>
@@ -417,8 +378,88 @@
 On fait le test avec filigranes</t>
   </si>
   <si>
-    <t>Lost of persistence on the server ?
-ZOUBIDA</t>
+    <t>DONE - Faire un github - Quentin
+DONE - Serveur Discord - Quentin
+DONE - Faire un point GitHub - Bonnes pratiques - Quentin
+Si 2 jours c'est trop =&gt; Commencer un POC
+Pourra servir pour la documentation du projet</t>
+  </si>
+  <si>
+    <t>Si il y a des échanges entre telle ou telle partie
+En discuter vendredi après les synthèses slides
+    - quel format ?
+    - quelle API? 
+    - confirmer les livrables</t>
+  </si>
+  <si>
+    <t>Documentation
+Revoir CNN</t>
+  </si>
+  <si>
+    <t>Cours julie Exo
+Transfer learning
+Debuter implantation de VGG ce jour
+Avoir un résult même si pas top</t>
+  </si>
+  <si>
+    <t>Pas encore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y a du tri à faire
+Insectes…
+</t>
+  </si>
+  <si>
+    <t>Modèle, modèle, modèle
+Reprendre les cours
+Commencer avec modèle simple</t>
+  </si>
+  <si>
+    <t>Recup peaux saines
+300
+Homogène aux autres catégories
+OneDrive
+Transfer très lent
+Elles sont toutes en 512x512 (très rapide)</t>
+  </si>
+  <si>
+    <t>Flask prise en main
+API flask
+Questions etc.</t>
+  </si>
+  <si>
+    <t>Tester API Flask
+On aura front &amp; API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09h30 - Point Aurélie - Philippe
+10H00 - SCRUM du matin
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09h30 - Point Aurélie - Dominique
+10H00 - SCRUM du matin
+1 ou 2 slides de présentation pour mettre ses idées à plat, les présenter à l'équipe :
+  Site Web &amp; API     - Quentin
+  Dataset &amp; modèle   - Dominique
+  Transfer Learning  - Patrice
+  Archi              - Philippe
+</t>
+  </si>
+  <si>
+    <t>Revoir MLFlow Tracking</t>
+  </si>
+  <si>
+    <t>MLFlow Project
+Idéalement déployer sur EC2 et sur GPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lost of persistence on the server ?
+</t>
+  </si>
+  <si>
+    <t>La perte de persistence est réglé
+Des soucis de syntaxe, d'incompatibilité Linux, WIN… des cours qui n'est vraiment pas clair.</t>
   </si>
 </sst>
 </file>
@@ -787,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -845,7 +886,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2090,15 +2130,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C2E7AC-1286-4FC1-84B0-DB92C81B15DE}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="127" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A7" zoomScale="89" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.5546875" customWidth="1"/>
+    <col min="3" max="3" width="81.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="103.88671875" customWidth="1"/>
     <col min="6" max="6" width="5.88671875" customWidth="1"/>
@@ -2106,13 +2146,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -2123,10 +2163,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="27">
+      <c r="A3" s="26">
         <v>18</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>45442</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -2138,7 +2178,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="28">
+      <c r="A4" s="27">
         <v>17</v>
       </c>
       <c r="B4" s="18">
@@ -2151,7 +2191,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="28">
+      <c r="A5" s="27">
         <v>16</v>
       </c>
       <c r="B5" s="18">
@@ -2159,12 +2199,12 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="28">
+      <c r="A6" s="27">
         <v>15</v>
       </c>
       <c r="B6" s="18">
@@ -2172,12 +2212,12 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="216" x14ac:dyDescent="0.3">
-      <c r="A7" s="28">
+      <c r="A7" s="27">
         <v>14</v>
       </c>
       <c r="B7" s="18">
@@ -2189,63 +2229,65 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A8" s="28">
+    <row r="8" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="27">
         <v>13</v>
       </c>
       <c r="B8" s="18">
         <v>45447</v>
       </c>
-      <c r="C8" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="47" t="s">
+      <c r="C8" s="41" t="s">
         <v>29</v>
       </c>
+      <c r="D8" s="46" t="s">
+        <v>28</v>
+      </c>
       <c r="E8" s="12" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
+      <c r="A9" s="27">
         <v>12</v>
       </c>
       <c r="B9" s="18">
         <v>45448</v>
       </c>
-      <c r="C9" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="48"/>
+      <c r="C9" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="47"/>
       <c r="E9" s="20"/>
     </row>
-    <row r="10" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>11</v>
       </c>
       <c r="B10" s="18">
         <v>45449</v>
       </c>
-      <c r="C10" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="49" t="s">
+      <c r="C10" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>10</v>
       </c>
       <c r="B11" s="18">
         <v>45450</v>
       </c>
-      <c r="C11" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="13"/>
+      <c r="C11" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
@@ -2255,8 +2297,8 @@
         <v>45451</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="44"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="43"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
@@ -2266,10 +2308,10 @@
         <v>45452</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="44"/>
+      <c r="E13" s="43"/>
     </row>
     <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
@@ -2278,10 +2320,10 @@
       <c r="B14" s="18">
         <v>45453</v>
       </c>
-      <c r="C14" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="50"/>
+      <c r="C14" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="49"/>
       <c r="E14" s="14" t="s">
         <v>26</v>
       </c>
@@ -2293,10 +2335,10 @@
       <c r="B15" s="18">
         <v>45454</v>
       </c>
-      <c r="C15" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="50"/>
+      <c r="C15" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="49"/>
       <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2306,10 +2348,10 @@
       <c r="B16" s="18">
         <v>45455</v>
       </c>
-      <c r="C16" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="51" t="s">
+      <c r="C16" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="50" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="15" t="s">
@@ -2323,10 +2365,10 @@
       <c r="B17" s="18">
         <v>45456</v>
       </c>
-      <c r="C17" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="52"/>
+      <c r="C17" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="51"/>
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
@@ -2336,10 +2378,10 @@
       <c r="B18" s="18">
         <v>45457</v>
       </c>
-      <c r="C18" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="53"/>
+      <c r="C18" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="52"/>
       <c r="E18" s="15" t="s">
         <v>23</v>
       </c>
@@ -2353,7 +2395,7 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="44" t="s">
+      <c r="E19" s="43" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2366,19 +2408,19 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="43" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="22">
+      <c r="A21" s="21">
         <v>0</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="22">
         <v>45460</v>
       </c>
-      <c r="C21" s="43" t="s">
-        <v>36</v>
+      <c r="C21" s="42" t="s">
+        <v>35</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>13</v>
@@ -2404,346 +2446,371 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.109375" customWidth="1"/>
     <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="39.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.88671875" customWidth="1"/>
     <col min="9" max="9" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="20.6640625" customWidth="1"/>
     <col min="13" max="13" width="68.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="55" t="s">
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="56" t="s">
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="57" t="s">
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="34" t="s">
+      <c r="K6" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="34" t="s">
+      <c r="L6" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="34" t="s">
+      <c r="M6" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="29">
+      <c r="A7" s="28">
         <v>45447</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="41" t="s">
+      <c r="E7" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="46" t="s">
+      <c r="M7" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="L7" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="M7" s="46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="29">
+    </row>
+    <row r="8" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="28">
         <v>45448</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
+      <c r="B8" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="45" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="29">
+      <c r="A9" s="28">
         <v>45449</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="29">
+      <c r="A10" s="28">
         <v>45450</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="29">
         <v>45451</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="29">
         <v>45452</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="29">
+      <c r="A13" s="28">
         <v>45453</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="29">
+      <c r="A14" s="28">
         <v>45454</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="29">
+      <c r="A15" s="28">
         <v>45455</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="29">
+      <c r="A16" s="28">
         <v>45456</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="29">
+      <c r="A17" s="28">
         <v>45457</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="30">
+      <c r="A18" s="29">
         <v>45458</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="30">
+      <c r="A19" s="29">
         <v>45459</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="29">
+      <c r="A20" s="28">
         <v>45460</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
update scrum et notes de meeting.
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="312" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A1630C4-4D3D-42F1-97CF-845D09EFBD1E}"/>
+  <xr:revisionPtr revIDLastSave="375" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{033AB8E5-9F43-4515-96E5-48910500A949}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -263,31 +263,6 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>10H45</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> : Après le point Aurélie - demo/POC - Inviter le prof
-Faire le point sur : 
- - ce qu'on a
- - ce qui nous manque
- - …</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
       <t>10H00</t>
     </r>
     <r>
@@ -316,27 +291,6 @@
 10H00 - SCRUM du matin</t>
   </si>
   <si>
-    <t>09h30 - Point Aurélie - Philippe
-10H00 - SCRUM du matin</t>
-  </si>
-  <si>
-    <t>09h30 - Point Aurélie - Dominique
-10H00 - SCRUM du matin</t>
-  </si>
-  <si>
-    <t>09h30 - Point Aurélie - Patrice
-10H00 - SCRUM du matin</t>
-  </si>
-  <si>
-    <t>09h30 - Point Aurélie - Philippe
-10H00 - SCRUM du matin AurélieTerminer l'archi des slides à midi?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09h30 - Point Aurélie - Dominique
-10H00 - SCRUM du matin
-Présentation l'après midi </t>
-  </si>
-  <si>
     <t>Doc &amp; Veille</t>
   </si>
   <si>
@@ -432,13 +386,24 @@
 On aura front &amp; API</t>
   </si>
   <si>
+    <t>Revoir MLFlow Tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lost of persistence on the server ?
+</t>
+  </si>
+  <si>
+    <t>La perte de persistence est réglé
+Des soucis de syntaxe, d'incompatibilité Linux, WIN… des cours qui n'est vraiment pas clair.</t>
+  </si>
+  <si>
     <t xml:space="preserve">09h30 - Point Aurélie - Philippe
-10H00 - SCRUM du matin
+10H15 - SCRUM du matin
 </t>
   </si>
   <si>
     <t xml:space="preserve">09h30 - Point Aurélie - Dominique
-10H00 - SCRUM du matin
+10H15 - SCRUM du matin
 1 ou 2 slides de présentation pour mettre ses idées à plat, les présenter à l'équipe :
   Site Web &amp; API     - Quentin
   Dataset &amp; modèle   - Dominique
@@ -447,19 +412,93 @@
 </t>
   </si>
   <si>
-    <t>Revoir MLFlow Tracking</t>
-  </si>
-  <si>
-    <t>MLFlow Project
-Idéalement déployer sur EC2 et sur GPU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lost of persistence on the server ?
+    <t>09h30 - Point Aurélie - Patrice
+10H15 - SCRUM du matin</t>
+  </si>
+  <si>
+    <t>09h30 - Point Aurélie - Philippe
+10H15 - SCRUM du matin</t>
+  </si>
+  <si>
+    <t>09h30 - Point Aurélie - Dominique
+10H15 - SCRUM du matin</t>
+  </si>
+  <si>
+    <t>09h30 - Point Aurélie - Philippe
+10H15 - SCRUM du matin AurélieTerminer l'archi des slides à midi?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09h30 - Point Aurélie - Dominique
+10H15 - SCRUM du matin
+Présentation l'après midi </t>
+  </si>
+  <si>
+    <t>Pas mal de perte de temps avec Project
+Un espace dans le path
+Image JEDHA obsoletes
+mflow pas à la meême version sur client et Tracking (crypto et paramiko)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLFlow Project en local
 </t>
   </si>
   <si>
-    <t>La perte de persistence est réglé
-Des soucis de syntaxe, d'incompatibilité Linux, WIN… des cours qui n'est vraiment pas clair.</t>
+    <t xml:space="preserve">MLFlow Project en local
+Plus de warning à l'execution
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revoir le cours sur le deep learning
+</t>
+  </si>
+  <si>
+    <t>2 slides pour demain</t>
+  </si>
+  <si>
+    <t>Commencer à entraîner un CNN sur le dataset
+2 slides pour demain</t>
+  </si>
+  <si>
+    <t>MLFLOW Project sur EC2
+Revoir user data, reboot et AMI
+MLFLOW Project sur GPU
+2 slides pour demain
+Refléchir aux use cases (gestion des mdp etc). Terraform? NGINX (reverse proxy…). Alternative à EC2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">NOTE comment on fait pour prévenir le/les TA? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+10H45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : Après le point Aurélie - demo/POC - Inviter le prof
+Faire le point sur : 
+ - ce qu'on a
+ - ce qui nous manque
+ - …</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -469,7 +508,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,6 +540,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -828,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -911,33 +956,6 @@
     <xf numFmtId="164" fontId="1" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -959,6 +977,27 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -981,16 +1020,16 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1804,6 +1843,157 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2011680</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3314700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="ZoneTexte 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{546AF50F-1E61-433D-1650-DD39085D9FA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="29199840" y="4686300"/>
+          <a:ext cx="4922520" cy="1447800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Messages</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> à passer Jeudi 6 juin</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>. Serveurs discord et Git en place</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>. Rétro planning en place depuis la semaine dernière</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>. Réunions SCRUM quotidiennes en place</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>. On est en train de terminer le sprint "DOC &amp; VEILLE"</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>. On v rentre dans le sprint "CODE 1/3"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>. Presentation de 2 slides par personne pour demain</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2130,8 +2320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C2E7AC-1286-4FC1-84B0-DB92C81B15DE}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="89" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="89" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2199,7 +2389,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="34" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2212,7 +2402,7 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="34" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2236,14 +2426,14 @@
       <c r="B8" s="18">
         <v>45447</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="46" t="s">
+      <c r="C8" s="32" t="s">
         <v>28</v>
       </c>
+      <c r="D8" s="44" t="s">
+        <v>27</v>
+      </c>
       <c r="E8" s="12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2253,26 +2443,26 @@
       <c r="B9" s="18">
         <v>45448</v>
       </c>
-      <c r="C9" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="47"/>
+      <c r="C9" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="45"/>
       <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="19">
+      <c r="A10" s="27">
         <v>11</v>
       </c>
       <c r="B10" s="18">
         <v>45449</v>
       </c>
-      <c r="C10" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="48" t="s">
+      <c r="C10" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="43"/>
     </row>
     <row r="11" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
@@ -2281,12 +2471,12 @@
       <c r="B11" s="18">
         <v>45450</v>
       </c>
-      <c r="C11" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="48"/>
+      <c r="C11" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="46"/>
       <c r="E11" s="13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2297,8 +2487,8 @@
         <v>45451</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
@@ -2308,24 +2498,24 @@
         <v>45452</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="43"/>
-    </row>
-    <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="E13" s="34"/>
+    </row>
+    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>7</v>
       </c>
       <c r="B14" s="18">
         <v>45453</v>
       </c>
-      <c r="C14" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="49"/>
+      <c r="C14" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="47"/>
       <c r="E14" s="14" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
@@ -2335,10 +2525,10 @@
       <c r="B15" s="18">
         <v>45454</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="49"/>
+      <c r="C15" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="47"/>
       <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2348,14 +2538,14 @@
       <c r="B16" s="18">
         <v>45455</v>
       </c>
-      <c r="C16" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="50" t="s">
+      <c r="C16" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="48" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2365,10 +2555,10 @@
       <c r="B17" s="18">
         <v>45456</v>
       </c>
-      <c r="C17" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="51"/>
+      <c r="C17" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="49"/>
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
@@ -2378,10 +2568,10 @@
       <c r="B18" s="18">
         <v>45457</v>
       </c>
-      <c r="C18" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="52"/>
+      <c r="C18" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="50"/>
       <c r="E18" s="15" t="s">
         <v>23</v>
       </c>
@@ -2395,7 +2585,7 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2408,7 +2598,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2419,8 +2609,8 @@
       <c r="B21" s="22">
         <v>45460</v>
       </c>
-      <c r="C21" s="42" t="s">
-        <v>35</v>
+      <c r="C21" s="33" t="s">
+        <v>58</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>13</v>
@@ -2446,83 +2636,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.88671875" customWidth="1"/>
-    <col min="9" max="9" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="20.6640625" customWidth="1"/>
-    <col min="13" max="13" width="68.5546875" customWidth="1"/>
+    <col min="2" max="13" width="52.77734375" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="54" t="s">
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="55" t="s">
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="56" t="s">
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="42" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2530,117 +2710,133 @@
       <c r="A7" s="28">
         <v>45447</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="40" t="s">
+      <c r="L7" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="M7" s="45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>45448</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="40" t="s">
+      <c r="B8" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="J8" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="44" t="s">
+      <c r="L8" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="L8" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="M8" s="45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>45449</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
+      <c r="B9" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>64</v>
+      </c>
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
+      <c r="G9" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>45450</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
       <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
@@ -2680,86 +2876,86 @@
       <c r="A13" s="28">
         <v>45453</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
       <c r="E13" s="35"/>
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="28">
         <v>45454</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="35"/>
       <c r="F14" s="35"/>
       <c r="G14" s="35"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
         <v>45455</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="35"/>
       <c r="F15" s="35"/>
       <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
         <v>45456</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
       <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>45457</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="35"/>
       <c r="F17" s="35"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
@@ -2799,18 +2995,18 @@
       <c r="A20" s="28">
         <v>45460</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="35"/>
       <c r="F20" s="35"/>
       <c r="G20" s="35"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Test EC2 et slides
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="375" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{033AB8E5-9F43-4515-96E5-48910500A949}"/>
+  <xr:revisionPtr revIDLastSave="425" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A28F0ED-7E6C-437E-AADD-1D3139A5A229}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -402,16 +402,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">09h30 - Point Aurélie - Dominique
-10H15 - SCRUM du matin
-1 ou 2 slides de présentation pour mettre ses idées à plat, les présenter à l'équipe :
-  Site Web &amp; API     - Quentin
-  Dataset &amp; modèle   - Dominique
-  Transfer Learning  - Patrice
-  Archi              - Philippe
-</t>
-  </si>
-  <si>
     <t>09h30 - Point Aurélie - Patrice
 10H15 - SCRUM du matin</t>
   </si>
@@ -450,9 +440,6 @@
   <si>
     <t xml:space="preserve">Revoir le cours sur le deep learning
 </t>
-  </si>
-  <si>
-    <t>2 slides pour demain</t>
   </si>
   <si>
     <t>Commencer à entraîner un CNN sur le dataset
@@ -499,6 +486,64 @@
  - ce qui nous manque
  - …</t>
     </r>
+  </si>
+  <si>
+    <t>Nom d'appli ?
+DermatoDetect
+SkinScan
+DermApp
+PhotoDerm
+SkinSage
+Dermis Diagnose
+SkinCheck : Philippe
+DermaSnap
+ClearSkin AI
+SpotCheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09h30 - Point Aurélie - Dominique
+10H15 - SCRUM du matin
+Choisir le nom de l'application
+1 ou 2 slides de présentation pour mettre ses idées à plat, les présenter à l'équipe :
+  Site Web &amp; API     - Quentin
+  Dataset &amp; modèle   - Dominique
+  Transfer Learning  - Patrice
+  Archi              - Philippe
+</t>
+  </si>
+  <si>
+    <t>No problemo à part les panneaux, insectes…
+Je vais y passer une heure ce jour
+Pas de peau saine</t>
+  </si>
+  <si>
+    <t>Doc + cours + recherche d'une solution sur Kaggle (suite recommendation de Dominique) + config d'une machine (locale) musclé et taillé pour les calculs cnn.
+DockerHub Image Tensorflow + GPU</t>
+  </si>
+  <si>
+    <t>Cours Transfer Learning
+Attnedre que le nettoyage soit terminé
+Prendre 3 images pour voir
+2 slides pour demain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 slides pour demain
+Commencer l'application web finale pour faire l'API propre
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai bien pris en main Flask coté API
+Test d'upload d'images par exemple </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai passé 1H avec Colin puis 1H30 avec Adrien. Pas de solution. A lafin avec Adrien on a peut être vu un truc. A tester ce matin. Adrien confirme qu'il n'a jamais vu de config EC2 d'élève tourner. </t>
+  </si>
+  <si>
+    <t>Essayer de deployer un MLproject sur EC2 et l'entrainer. Les 2 slides pour ce matin.</t>
+  </si>
+  <si>
+    <t>EC2 aujourd'hui
+Essyer de trouver une alternative à EC22 ce WE.</t>
   </si>
 </sst>
 </file>
@@ -1846,15 +1891,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2011680</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>2125980</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>3314700</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:colOff>3429000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1869,8 +1914,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29199840" y="4686300"/>
-          <a:ext cx="4922520" cy="1447800"/>
+          <a:off x="29314140" y="7452360"/>
+          <a:ext cx="4922520" cy="2606040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1925,6 +1970,28 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
+            <a:t>. On est en train de terminer le sprint "DOC &amp; VEILLE"</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>. On v rentre dans le sprint "CODE 1/3"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
             <a:t>. Serveurs discord et Git en place</a:t>
           </a:r>
         </a:p>
@@ -1956,7 +2023,49 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>. On est en train de terminer le sprint "DOC &amp; VEILLE"</a:t>
+            <a:t>. Data set partagé (pas encore sur S3)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>. Presentation de 2 slides par personne pour demain</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Info Aurélie</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Passez du temps sur l'evaluation du model</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Ses performances, ses limites ?</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="fr-FR" sz="1100" baseline="0">
@@ -1969,17 +2078,53 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>. On v rentre dans le sprint "CODE 1/3"</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>. Presentation de 2 slides par personne pour demain</a:t>
-          </a:r>
+            <a:t>Quel metrique? Pourquoi ?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Quid du preprocessing</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>10% déploiement, 80% analyse jeu de données</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
@@ -2320,8 +2465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C2E7AC-1286-4FC1-84B0-DB92C81B15DE}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="89" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A7" zoomScale="89" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2464,7 +2609,7 @@
       </c>
       <c r="E10" s="43"/>
     </row>
-    <row r="11" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -2472,7 +2617,7 @@
         <v>45450</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="13" t="s">
@@ -2511,11 +2656,11 @@
         <v>45453</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" s="47"/>
       <c r="E14" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
@@ -2526,7 +2671,7 @@
         <v>45454</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="47"/>
       <c r="E15" s="14"/>
@@ -2539,7 +2684,7 @@
         <v>45455</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="48" t="s">
         <v>11</v>
@@ -2556,7 +2701,7 @@
         <v>45456</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="16"/>
@@ -2569,7 +2714,7 @@
         <v>45457</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="50"/>
       <c r="E18" s="15" t="s">
@@ -2610,7 +2755,7 @@
         <v>45460</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>13</v>
@@ -2636,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2776,7 +2921,7 @@
         <v>51</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K8" s="36" t="s">
         <v>47</v>
@@ -2788,40 +2933,48 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>45449</v>
       </c>
       <c r="B9" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
+      <c r="E9" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>33</v>
+      </c>
       <c r="G9" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" s="30" t="s">
+      <c r="K9" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="L9" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
       <c r="M9" s="36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>45450</v>
       </c>
@@ -2831,9 +2984,15 @@
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
       <c r="G10" s="35"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="H10" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>74</v>
+      </c>
       <c r="K10" s="36"/>
       <c r="L10" s="36"/>
       <c r="M10" s="36"/>

</xml_diff>

<commit_message>
premier run sous skincheck
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="425" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A28F0ED-7E6C-437E-AADD-1D3139A5A229}"/>
+  <xr:revisionPtr revIDLastSave="451" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89967C7A-37CE-4248-8865-D25530131941}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -488,19 +488,6 @@
     </r>
   </si>
   <si>
-    <t>Nom d'appli ?
-DermatoDetect
-SkinScan
-DermApp
-PhotoDerm
-SkinSage
-Dermis Diagnose
-SkinCheck : Philippe
-DermaSnap
-ClearSkin AI
-SpotCheck</t>
-  </si>
-  <si>
     <t xml:space="preserve">09h30 - Point Aurélie - Dominique
 10H15 - SCRUM du matin
 Choisir le nom de l'application
@@ -536,14 +523,89 @@
 Test d'upload d'images par exemple </t>
   </si>
   <si>
-    <t xml:space="preserve">J'ai passé 1H avec Colin puis 1H30 avec Adrien. Pas de solution. A lafin avec Adrien on a peut être vu un truc. A tester ce matin. Adrien confirme qu'il n'a jamais vu de config EC2 d'élève tourner. </t>
-  </si>
-  <si>
     <t>Essayer de deployer un MLproject sur EC2 et l'entrainer. Les 2 slides pour ce matin.</t>
   </si>
   <si>
+    <t>Ai cherché des peaux sombres
+Rien rajouté (faut les mêmes classes)
+On verra à la fin car y a du boulot</t>
+  </si>
+  <si>
+    <t>Galère pour récupérer le zip (dataset) vers COLAB. On va rien… On a un logo de progression au bout de 20 min. 
+Entrainement lent</t>
+  </si>
+  <si>
+    <t>Entrainement
+Aurélie veut voir les scores. 
+Peur qu'on sorte pas les bons score et qu'on brasse du vent.
+En classification on devrait suivre F1 score mais pas que… Matrice de confusion, Grad Cam : couche en sortie de rsx. Permet de voir si le modèle focus là où faut.</t>
+  </si>
+  <si>
+    <t>Lecture de papiers/articles scoring etc. utilisés sur malanome
+Je suis au tout début du transfer learning
+Grad Cam : parait cohérent</t>
+  </si>
+  <si>
+    <t>Matin : metric et dominique
+Après midi : Lecture cours puis tests</t>
+  </si>
+  <si>
+    <t>Galère pour télécharger images
+COLAB à jour mais lent
+Ma machine : rapide mais soucis de version</t>
+  </si>
+  <si>
+    <t>Application finale
+API
+Front
+Modèle en local tout basique (retourne 0)
+API et App dev en //</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nom d'appli ?
+DermatoDetect
+SkinScan
+DermApp
+PhotoDerm
+SkinSage
+Dermis Diagnose
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SkinCheck</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : Philippe Domin Patrice Quent
+DermaSnap
+ClearSkin AI
+SpotCheck</t>
+    </r>
+  </si>
+  <si>
+    <t>Faire un predict sur Heroku
+skincheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai passé 1H avec Colin puis 1H30 avec Adrien. Pas de solution. A la fin avec Adrien on a peut être vu un truc. A tester ce matin. Adrien confirme qu'il n'a jamais vu de config EC2 d'élève tourner. </t>
+  </si>
+  <si>
     <t>EC2 aujourd'hui
-Essyer de trouver une alternative à EC22 ce WE.</t>
+Essayer de trouver une alternative à EC22 ce WE.
+Voir Raphael</t>
   </si>
 </sst>
 </file>
@@ -2617,7 +2679,7 @@
         <v>45450</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="13" t="s">
@@ -2781,8 +2843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2941,19 +3003,19 @@
         <v>61</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>62</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="35" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H9" s="30" t="s">
         <v>60</v>
@@ -2965,37 +3027,55 @@
         <v>63</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L9" s="36" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="M9" s="36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>45450</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="B10" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>76</v>
+      </c>
       <c r="H10" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
+        <v>82</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="36" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="29">

</xml_diff>

<commit_message>
Travail du WE. Templates, debug etc.
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="451" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89967C7A-37CE-4248-8865-D25530131941}"/>
+  <xr:revisionPtr revIDLastSave="459" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F8D25F0-6ACC-4524-B189-E3732E1390D0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -606,6 +606,17 @@
     <t>EC2 aujourd'hui
 Essayer de trouver une alternative à EC22 ce WE.
 Voir Raphael</t>
+  </si>
+  <si>
+    <t>Ai tout remonté en utilisant le nom du projet : Skin Check</t>
+  </si>
+  <si>
+    <t>J'arrive enfin à envoyer 1 et 1 seul jeu de paramètres sur Heroku et Artifacts. Sombre histoire de MLFLOW_EXPERIMENT_NAME et de MLFLOW_EXPERIMENT_ID. Pas mal de tests pour comprendre comment mlflow fonctionne et comment allèger le fichier secrets.ps1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importation d'images sur S3 pour tester
+Template de train.py sklearn
+</t>
   </si>
 </sst>
 </file>
@@ -2843,8 +2854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="F9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3077,7 +3088,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>45451</v>
       </c>
@@ -3087,14 +3098,18 @@
       <c r="E11" s="38"/>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
+      <c r="H11" s="38" t="s">
+        <v>83</v>
+      </c>
       <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="J11" s="38" t="s">
+        <v>84</v>
+      </c>
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
       <c r="M11" s="38"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>45452</v>
       </c>
@@ -3106,7 +3121,9 @@
       <c r="G12" s="38"/>
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="J12" s="38" t="s">
+        <v>85</v>
+      </c>
       <c r="K12" s="38"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>

</xml_diff>

<commit_message>
update suite pb git
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="425" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A28F0ED-7E6C-437E-AADD-1D3139A5A229}"/>
+  <xr:revisionPtr revIDLastSave="462" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A07228-E216-4ADC-9EA7-6672025D3F9D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -488,19 +488,6 @@
     </r>
   </si>
   <si>
-    <t>Nom d'appli ?
-DermatoDetect
-SkinScan
-DermApp
-PhotoDerm
-SkinSage
-Dermis Diagnose
-SkinCheck : Philippe
-DermaSnap
-ClearSkin AI
-SpotCheck</t>
-  </si>
-  <si>
     <t xml:space="preserve">09h30 - Point Aurélie - Dominique
 10H15 - SCRUM du matin
 Choisir le nom de l'application
@@ -536,14 +523,106 @@
 Test d'upload d'images par exemple </t>
   </si>
   <si>
-    <t xml:space="preserve">J'ai passé 1H avec Colin puis 1H30 avec Adrien. Pas de solution. A lafin avec Adrien on a peut être vu un truc. A tester ce matin. Adrien confirme qu'il n'a jamais vu de config EC2 d'élève tourner. </t>
-  </si>
-  <si>
     <t>Essayer de deployer un MLproject sur EC2 et l'entrainer. Les 2 slides pour ce matin.</t>
   </si>
   <si>
+    <t>Ai cherché des peaux sombres
+Rien rajouté (faut les mêmes classes)
+On verra à la fin car y a du boulot</t>
+  </si>
+  <si>
+    <t>Galère pour récupérer le zip (dataset) vers COLAB. On va rien… On a un logo de progression au bout de 20 min. 
+Entrainement lent</t>
+  </si>
+  <si>
+    <t>Entrainement
+Aurélie veut voir les scores. 
+Peur qu'on sorte pas les bons score et qu'on brasse du vent.
+En classification on devrait suivre F1 score mais pas que… Matrice de confusion, Grad Cam : couche en sortie de rsx. Permet de voir si le modèle focus là où faut.</t>
+  </si>
+  <si>
+    <t>Lecture de papiers/articles scoring etc. utilisés sur malanome
+Je suis au tout début du transfer learning
+Grad Cam : parait cohérent</t>
+  </si>
+  <si>
+    <t>Matin : metric et dominique
+Après midi : Lecture cours puis tests</t>
+  </si>
+  <si>
+    <t>Galère pour télécharger images
+COLAB à jour mais lent
+Ma machine : rapide mais soucis de version</t>
+  </si>
+  <si>
+    <t>Application finale
+API
+Front
+Modèle en local tout basique (retourne 0)
+API et App dev en //</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nom d'appli ?
+DermatoDetect
+SkinScan
+DermApp
+PhotoDerm
+SkinSage
+Dermis Diagnose
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SkinCheck</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : Philippe Domin Patrice Quent
+DermaSnap
+ClearSkin AI
+SpotCheck</t>
+    </r>
+  </si>
+  <si>
+    <t>Faire un predict sur Heroku
+skincheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai passé 1H avec Colin puis 1H30 avec Adrien. Pas de solution. A la fin avec Adrien on a peut être vu un truc. A tester ce matin. Adrien confirme qu'il n'a jamais vu de config EC2 d'élève tourner. </t>
+  </si>
+  <si>
     <t>EC2 aujourd'hui
-Essyer de trouver une alternative à EC22 ce WE.</t>
+Essayer de trouver une alternative à EC22 ce WE.
+Voir Raphael</t>
+  </si>
+  <si>
+    <t>Ai tout remonté en utilisant le nom du projet : Skin Check</t>
+  </si>
+  <si>
+    <t>J'arrive enfin à envoyer 1 et 1 seul jeu de paramètres sur Heroku et Artifacts. Sombre histoire de MLFLOW_EXPERIMENT_NAME et de MLFLOW_EXPERIMENT_ID. Pas mal de tests pour comprendre comment mlflow fonctionne et comment allèger le fichier secrets.ps1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importation d'images sur S3 pour tester
+Template de train.py sklearn
+</t>
+  </si>
+  <si>
+    <t>Terminer les templates sklearn et TF
+Test des template training local
+Un peu de doc
+Essais sur EC2 (encore!)</t>
   </si>
 </sst>
 </file>
@@ -2617,7 +2696,7 @@
         <v>45450</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="13" t="s">
@@ -2781,8 +2860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="F9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2941,19 +3020,19 @@
         <v>61</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>62</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="35" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H9" s="30" t="s">
         <v>60</v>
@@ -2965,39 +3044,57 @@
         <v>63</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L9" s="36" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="M9" s="36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>45450</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="B10" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>76</v>
+      </c>
       <c r="H10" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>45451</v>
       </c>
@@ -3007,14 +3104,18 @@
       <c r="E11" s="38"/>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
+      <c r="H11" s="38" t="s">
+        <v>83</v>
+      </c>
       <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="J11" s="38" t="s">
+        <v>84</v>
+      </c>
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
       <c r="M11" s="38"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>45452</v>
       </c>
@@ -3026,12 +3127,14 @@
       <c r="G12" s="38"/>
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="J12" s="38" t="s">
+        <v>85</v>
+      </c>
       <c r="K12" s="38"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
         <v>45453</v>
       </c>
@@ -3041,7 +3144,9 @@
       <c r="E13" s="35"/>
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
-      <c r="H13" s="30"/>
+      <c r="H13" s="30" t="s">
+        <v>86</v>
+      </c>
       <c r="I13" s="30"/>
       <c r="J13" s="30"/>
       <c r="K13" s="36"/>

</xml_diff>

<commit_message>
Test TF avec image TF GPU
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="459" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F8D25F0-6ACC-4524-B189-E3732E1390D0}"/>
+  <xr:revisionPtr revIDLastSave="462" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A07228-E216-4ADC-9EA7-6672025D3F9D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -617,6 +617,12 @@
     <t xml:space="preserve">Importation d'images sur S3 pour tester
 Template de train.py sklearn
 </t>
+  </si>
+  <si>
+    <t>Terminer les templates sklearn et TF
+Test des template training local
+Un peu de doc
+Essais sur EC2 (encore!)</t>
   </si>
 </sst>
 </file>
@@ -2213,10 +2219,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2855,7 +2857,7 @@
   <dimension ref="A5:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3128,7 +3130,7 @@
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
         <v>45453</v>
       </c>
@@ -3138,7 +3140,9 @@
       <c r="E13" s="35"/>
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
-      <c r="H13" s="30"/>
+      <c r="H13" s="30" t="s">
+        <v>86</v>
+      </c>
       <c r="I13" s="30"/>
       <c r="J13" s="30"/>
       <c r="K13" s="36"/>

</xml_diff>

<commit_message>
Ai avancé sur le test predict()
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="462" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A07228-E216-4ADC-9EA7-6672025D3F9D}"/>
+  <xr:revisionPtr revIDLastSave="549" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{017A44DC-1B8B-4382-8189-DF682AD46666}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -203,81 +203,11 @@
     <t>Issues</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>12H00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> : demo/POC  - Inviter le prof
-Faire le point sur : 
- - ce qu'on a
- - ce qui nous manque
- - …
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>18H00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> : Fournir les données, graphes, captures écrans pour les slides</t>
-    </r>
-  </si>
-  <si>
     <t>Architecture study
 Course review</t>
   </si>
   <si>
     <t>Finish course review</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>10H00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> : Après le point Aurélie - demo/POC - Inviter le prof
-Faire le point sur : 
- - ce qu'on a
- - ce qui nous manque
- - …</t>
-    </r>
   </si>
   <si>
     <t>DOC-VEILLE</t>
@@ -410,19 +340,6 @@
 10H15 - SCRUM du matin</t>
   </si>
   <si>
-    <t>09h30 - Point Aurélie - Dominique
-10H15 - SCRUM du matin</t>
-  </si>
-  <si>
-    <t>09h30 - Point Aurélie - Philippe
-10H15 - SCRUM du matin AurélieTerminer l'archi des slides à midi?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09h30 - Point Aurélie - Dominique
-10H15 - SCRUM du matin
-Présentation l'après midi </t>
-  </si>
-  <si>
     <t>Pas mal de perte de temps avec Project
 Un espace dans le path
 Image JEDHA obsoletes
@@ -451,41 +368,6 @@
 MLFLOW Project sur GPU
 2 slides pour demain
 Refléchir aux use cases (gestion des mdp etc). Terraform? NGINX (reverse proxy…). Alternative à EC2</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">NOTE comment on fait pour prévenir le/les TA? </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-10H45</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> : Après le point Aurélie - demo/POC - Inviter le prof
-Faire le point sur : 
- - ce qu'on a
- - ce qui nous manque
- - …</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">09h30 - Point Aurélie - Dominique
@@ -624,6 +506,147 @@
 Un peu de doc
 Essais sur EC2 (encore!)</t>
   </si>
+  <si>
+    <t>Faire getting-started pour aider Dominique et Patrice à démarrer avec les templates de code.</t>
+  </si>
+  <si>
+    <t>09h30 - Point Aurélie - Dominique
+10H15 - SCRUM du matin
+18H00 - Ebauche de slides</t>
+  </si>
+  <si>
+    <t>09h30 - Point Aurélie - Patrice - Feedback sur les slides
+10H15 - SCRUM du matin
+??H?? - Prévoir une répétition à blanc</t>
+  </si>
+  <si>
+    <t>09h30 - Point Aurélie - Philippe
+10H15 - SCRUM du matin Aurélie
+??H?? - Répétition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matin - TA
+Après midi - Aurélie
+09H30, - SCRUM du matin
+Présentation l'après midi </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>10H00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : Après le point Aurélie - demo/POC - Inviter le prof?
+Faire le point sur : 
+ - ce qu'on a
+ - ce qui nous manque
+ - …</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>12H00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : demo/POC  - Inviter le prof?
+Faire le point sur : 
+ - ce qu'on a
+ - ce qui nous manque
+ - …
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>18H00</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : Fournir les données, graphes, captures écrans pour les slides</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">NOTE comment on fait pour prévenir le/les TA? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+10H45</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> : Après le point Aurélie - demo/POC - Inviter le prof
+Faire le point sur : 
+ - ce qu'on a
+ - ce qui nous manque
+ - …</t>
+    </r>
+  </si>
+  <si>
+    <t>Les templates fonctionnent avec les images TensorFlow GPU. 
+Vérification de la configuration pour utiliser le GPU.
+Vérification accès public serveur mlflow tracking
+Test d'invocation de la méthode predict() sur le serveur mlflow-tracking
+Slide archi pour Jeudi</t>
+  </si>
 </sst>
 </file>
 
@@ -632,7 +655,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,6 +692,15 @@
     </font>
     <font>
       <b/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
       <sz val="11"/>
       <name val="Courier New"/>
       <family val="3"/>
@@ -997,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1154,6 +1186,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1969,16 +2004,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>2125980</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3589020</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>3429000</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3558540</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1993,8 +2028,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29314140" y="7452360"/>
-          <a:ext cx="4922520" cy="2606040"/>
+          <a:off x="23538180" y="11742420"/>
+          <a:ext cx="10835640" cy="7353300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2028,6 +2063,935 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Message à passer Mardi 11 06 ----------------------------</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Dominique : </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Call avec Aurélie &amp; Patrice</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Call avec Patrice &amp; Philippe</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Entrainement d'un CNN (résultats restent décevants)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Aujourd'hui : envie d'intégrer une data augmentation (je sais qu'Aurélie n'est pas fan) pour voir ce que ça donne.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:prstClr val="black"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Patrice : </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:prstClr val="black"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Quentin :</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:prstClr val="black"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Philippe :</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>On peut logguer sur MLFlow-Tracking à partir d'une image TensorFlow GPU (utilisée Patrice &amp; Dominique) </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Vérification de la configuration pour vraiment utiliser les GPU</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Vérification accès public mlflow tracking (j'avais un doute)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Invocation de predict() sur le serveur mlflow-tracking</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Slide archi pour Jeudi</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:prstClr val="black"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:prstClr val="black"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Info Aurélie du Lundi 10 06 ----------------------------</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:prstClr val="black"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Mercredi soir    : Ebauche slide envoyée Aurélie</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Jeudi matin      : Feedback </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Jeudi (?)        : Répéter à blanc avant vendredi matin</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Vendredi matin   : 1ere répétition</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Lundi matin      : TA</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Lundi après midi : Aurélie</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" b="1">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" b="1">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -2040,7 +3004,7 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t> à passer Jeudi 6 juin</a:t>
+            <a:t> à passer Jeudi 6 juin ----------------------------</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2219,6 +3183,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2540,8 +3508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C2E7AC-1286-4FC1-84B0-DB92C81B15DE}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="89" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A9" zoomScale="89" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2647,13 +3615,13 @@
         <v>45447</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2664,7 +3632,7 @@
         <v>45448</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="45"/>
       <c r="E9" s="20"/>
@@ -2677,7 +3645,7 @@
         <v>45449</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="46" t="s">
         <v>10</v>
@@ -2685,22 +3653,22 @@
       <c r="E10" s="43"/>
     </row>
     <row r="11" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
+      <c r="A11" s="27">
         <v>10</v>
       </c>
       <c r="B11" s="18">
         <v>45450</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
+      <c r="A12" s="27">
         <v>9</v>
       </c>
       <c r="B12" s="18">
@@ -2711,7 +3679,7 @@
       <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="19">
+      <c r="A13" s="27">
         <v>8</v>
       </c>
       <c r="B13" s="18">
@@ -2724,18 +3692,18 @@
       <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="19">
+      <c r="A14" s="27">
         <v>7</v>
       </c>
       <c r="B14" s="18">
         <v>45453</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" s="47"/>
-      <c r="E14" s="14" t="s">
-        <v>64</v>
+      <c r="E14" s="55" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
@@ -2746,7 +3714,7 @@
         <v>45454</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D15" s="47"/>
       <c r="E15" s="14"/>
@@ -2759,16 +3727,16 @@
         <v>45455</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="D16" s="48" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>4</v>
       </c>
@@ -2776,7 +3744,7 @@
         <v>45456</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="16"/>
@@ -2789,11 +3757,11 @@
         <v>45457</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="D18" s="50"/>
       <c r="E18" s="15" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -2830,7 +3798,7 @@
         <v>45460</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>13</v>
@@ -2856,14 +3824,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="F18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="52.77734375" style="39" customWidth="1"/>
+    <col min="2" max="7" width="52.77734375" style="39" customWidth="1"/>
+    <col min="8" max="8" width="105.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="52.77734375" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2931,40 +3901,40 @@
         <v>45447</v>
       </c>
       <c r="B7" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="35" t="s">
+      <c r="M7" s="36" t="s">
         <v>35</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="36" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -2972,40 +3942,40 @@
         <v>45448</v>
       </c>
       <c r="B8" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="36" t="s">
         <v>46</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="K8" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" s="36" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
@@ -3013,40 +3983,40 @@
         <v>45449</v>
       </c>
       <c r="B9" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="31" t="s">
+      <c r="F9" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>68</v>
-      </c>
       <c r="H9" s="30" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I9" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="K9" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="M9" s="36" t="s">
         <v>63</v>
-      </c>
-      <c r="K9" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="M9" s="36" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -3054,40 +4024,40 @@
         <v>45450</v>
       </c>
       <c r="B10" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="31" t="s">
+      <c r="L10" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="36" t="s">
         <v>74</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="K10" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="L10" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" s="36" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -3101,11 +4071,11 @@
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
       <c r="H11" s="38" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I11" s="38"/>
       <c r="J11" s="38" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
@@ -3124,7 +4094,7 @@
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K12" s="38"/>
       <c r="L12" s="38"/>
@@ -3141,15 +4111,17 @@
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
       <c r="H13" s="30" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
+      <c r="J13" s="30" t="s">
+        <v>81</v>
+      </c>
       <c r="K13" s="36"/>
       <c r="L13" s="36"/>
       <c r="M13" s="36"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="28">
         <v>45454</v>
       </c>
@@ -3159,7 +4131,9 @@
       <c r="E14" s="35"/>
       <c r="F14" s="35"/>
       <c r="G14" s="35"/>
-      <c r="H14" s="30"/>
+      <c r="H14" s="30" t="s">
+        <v>89</v>
+      </c>
       <c r="I14" s="30"/>
       <c r="J14" s="30"/>
       <c r="K14" s="36"/>

</xml_diff>

<commit_message>
Update du modeles et test.
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="855" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEA916D5-9BF1-457E-B087-D275E73B090C}"/>
+  <xr:revisionPtr revIDLastSave="895" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5CCEFFC-F146-4CA1-B649-D71E8EDEE5D2}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="3132" windowWidth="23040" windowHeight="14244" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
   <si>
     <t>Date</t>
   </si>
@@ -728,6 +728,94 @@
 Les modeles se suivent et se ressemblent
 Si besoin demain je réduis. Sinon je passe en tranfer</t>
     </r>
+  </si>
+  <si>
+    <t>1 - Soucis Git et EC2 (toujours et encore)
+2 - EC2 - Finalement call prévu avec Greg demain
+3 - Ai regardé RunPod.io (alternative à EC2?). Pas tout compris à part qu'il fallait que je paie encore. Call Adrien demain ? Standby pour l'instant.
+Partie 2/n
+4 - Concernant les models... Heu je veux bien aider et rentrer dans la danse mais j'arrive avec 9 jours de retard... J'ai lu un peu. Ai voulu jeter un oeil sur le code de transfer learning de Patrice mais je l'ai reçu un peu tard sur GitHub (23H30). En plus je comprends pas tout ce qui est fait... Je me demande si demain après midi ca vaudrait pas le coup que Patrice nous présente (à toi et moi par exemple) son code de transfer learning (.py ou .ipynb on s'en fout on s'adaptera toujours). Faudra voir demain. By the way, je me demande si on pourrait pas essayer de faire du transfer learning avec un autre modèle histoire de varier les plaisirs : EfficientNetB7 ou ResNet101V2 par exemple. Pour l'instant dans le code de Patrice c'est du InceptionV3 je crois. A discuter. Encore une fois, je découvre le sujet et on est mercredi... En tout cas si je lance des runs les résultats et artifacts iront sur le serveur mlflow tracking dès le départ.
+5 - Ai regardé comment ajouter des images dans les artifacts de mlflow tracking (matrice de confusion par exemple)
+6 - Ai finalisé le slide archi (mais pas partagé sur github because j'ai peur de tout casser pour la 53eme fois)
+7 - Call avec Patrice qui avait des questions mlflow tracking (support jupyter notebook)
+8 - J'ai pas l'occasion de reparler des prédiction avec Quentin. J'imagine que tout tourne de son côté.
+9 - En attendant le code de Patrice, je suis revenu ce soir sur un bout de code flask qui date de ce WE : on choisit une image, elle s'affiche, on peut zoomer et  sélectionner une zone d'interêt avant de ne garder qu'une image 512x512.
+10 - Un modèle de transfer learning fonctionne
+Accuracy: 0.0694
+Precision: 0.0634
+Recall: 0.0694
+F1 Score: 0.0576</t>
+  </si>
+  <si>
+    <t>Voir sensibilité = capacité du test à bien détecter les gens vraiment malades.
+On peut pas utiliser la sensibilité toute seule.
+Regarder aussi specificté
+La sensibilité correspond à la probabilité d'être testé positif lorsqu'on est malade : La spécificité correspond à la probabilité d'être testé négatif lorsqu'on n'est pas malade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fine tuning
+Je cherche à améliorer la loss et accuracy
+Accuracy = 0.2 puis = 0.5
+Loss = ??
+</t>
+  </si>
+  <si>
+    <t>Aurélie indique
+Etape 1 : Accuracy &amp; F1 score*
+Etape 2 : Ensuite les autres metrique</t>
+  </si>
+  <si>
+    <t>Regarder F1 score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'arrive pas à logguer les matrices de confusion
+J'overfit pas mal
+</t>
+  </si>
+  <si>
+    <t>Je travaille sur moins de classes
+3 classes à la fin
+couche de convolution en plus
+La loss baisse puis Plateau 
+25 epochs
+Je commence à overfitter
+Je peux encore baisser (15 epochs)
+Je suis à 20 min 3 classes
+Validation
+Accuracy = 0,6 epoch 8
+Loss = 0,8 epoch 8</t>
+  </si>
+  <si>
+    <t>1 - Le modèle InceptionV3 (brut de fonderie) envoit ses courbes, matrices, paramètres, résultats et benchs sur mlflow tracking
+2 - Slides relus et envoyés avant minuit</t>
+  </si>
+  <si>
+    <t>EC2 &amp; Git</t>
+  </si>
+  <si>
+    <t>Revoir les slides et l'histoire. Le faire passer sur Google (attention animations). Prévoir un pdf ?
+Point technos avec la dream team
+Entre temps, faire tourner le modèle pour diminuer l'overfit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas de réunion SCRUM hier
+Répétiion en fin de journée 
+Modification du modèle
+Ajout d'une fonction Early_Stopping
+A la sortie du InceptionV3
+Supprimer la couche GlobalAveragePooling2D et ajout d'une couche Flaten
+Ajout d'une regulation L2 =&gt; Test associés
+Ajout de 2 couches dense 1024 et 512 =&gt; Test associés
+</t>
+  </si>
+  <si>
+    <t>Répétition à 9H40
+Convertir les slides
+Bien comprendre la nature des paramètres accuracy etc. qui sont sortis. C'est du train, valiadtion, pourquoi c'est si différent des graphes?
+Continuer à jourer avec le modèle
+Dégeler des lots de 4 couches jusqu'à 10% du modèle InceptionV3 et voir ce que cela donne
+22 Mds de paramètres dans 311 couches actuellement
+Changer de modèle ?</t>
   </si>
 </sst>
 </file>
@@ -4053,8 +4141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="G15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4062,7 +4150,8 @@
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="52.77734375" style="39" customWidth="1"/>
     <col min="8" max="8" width="105.6640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="52.77734375" style="39" customWidth="1"/>
+    <col min="9" max="9" width="52.77734375" style="39" customWidth="1"/>
+    <col min="10" max="10" width="80" style="39" customWidth="1"/>
     <col min="11" max="11" width="102.109375" style="39" customWidth="1"/>
     <col min="12" max="13" width="52.77734375" style="39" customWidth="1"/>
   </cols>
@@ -4401,24 +4490,38 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
         <v>45455</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
+      <c r="B15" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>107</v>
+      </c>
       <c r="D15" s="31"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="30"/>
+      <c r="E15" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>104</v>
+      </c>
       <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
+      <c r="J15" s="30" t="s">
+        <v>105</v>
+      </c>
       <c r="K15" s="36"/>
       <c r="L15" s="36"/>
       <c r="M15" s="36"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
         <v>45456</v>
       </c>
@@ -4428,14 +4531,20 @@
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
       <c r="G16" s="35"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="H16" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="J16" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="K16" s="36"/>
       <c r="L16" s="36"/>
       <c r="M16" s="36"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>45457</v>
       </c>
@@ -4445,9 +4554,15 @@
       <c r="E17" s="35"/>
       <c r="F17" s="35"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
+      <c r="H17" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>115</v>
+      </c>
       <c r="K17" s="36"/>
       <c r="L17" s="36"/>
       <c r="M17" s="36"/>

</xml_diff>

<commit_message>
relecture - ajout image archi
</commit_message>
<xml_diff>
--- a/admin/skin_project.xlsx
+++ b/admin/skin_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/Formations_JEDHA/skin_project/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="895" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5CCEFFC-F146-4CA1-B649-D71E8EDEE5D2}"/>
+  <xr:revisionPtr revIDLastSave="900" documentId="8_{AFC0C9B4-C45E-4A88-AE41-5C8E4C8F3B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1127EF37-33F9-401F-8019-3E4321E450A6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{A33F6934-330D-448E-A98A-4C648D54B491}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="119">
   <si>
     <t>Date</t>
   </si>
@@ -816,6 +816,22 @@
 Dégeler des lots de 4 couches jusqu'à 10% du modèle InceptionV3 et voir ce que cela donne
 22 Mds de paramètres dans 311 couches actuellement
 Changer de modèle ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisation nettoyage des répertoires
+Documentation. Relire et m'assurer que les instructions sont up to date
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas mal de temps passé sur le "bug" des confusion matrcices
+C'est bon c'est réglé
+</t>
+  </si>
+  <si>
+    <t>Je me suis fait un petit bout de code qui envoie un mail quand les tests sont terminés
+Ai lancé 1 ou 2 run historie de
+Répétition le matin
+Présentation du projet l'après midi</t>
   </si>
 </sst>
 </file>
@@ -4141,8 +4157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612ACBE-B8E7-421B-9F4C-27BD14431655}">
   <dimension ref="A5:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="F14" zoomScale="78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4380,7 +4396,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>45451</v>
       </c>
@@ -4521,7 +4537,7 @@
       <c r="L15" s="36"/>
       <c r="M15" s="36"/>
     </row>
-    <row r="16" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
         <v>45456</v>
       </c>
@@ -4567,7 +4583,7 @@
       <c r="L17" s="36"/>
       <c r="M17" s="36"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>45458</v>
       </c>
@@ -4577,14 +4593,16 @@
       <c r="E18" s="38"/>
       <c r="F18" s="38"/>
       <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
+      <c r="H18" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="I18" s="38"/>
       <c r="J18" s="38"/>
       <c r="K18" s="38"/>
       <c r="L18" s="38"/>
       <c r="M18" s="38"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="29">
         <v>45459</v>
       </c>
@@ -4594,14 +4612,16 @@
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
       <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+      <c r="H19" s="38" t="s">
+        <v>117</v>
+      </c>
       <c r="I19" s="38"/>
       <c r="J19" s="38"/>
       <c r="K19" s="38"/>
       <c r="L19" s="38"/>
       <c r="M19" s="38"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
         <v>45460</v>
       </c>
@@ -4613,7 +4633,9 @@
       <c r="G20" s="35"/>
       <c r="H20" s="30"/>
       <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="J20" s="30" t="s">
+        <v>118</v>
+      </c>
       <c r="K20" s="36"/>
       <c r="L20" s="36"/>
       <c r="M20" s="36"/>

</xml_diff>